<commit_message>
added CIs in Output table via verbose_ci and CIs will be exported, updated Readme, update xlsx file parameter returns
</commit_message>
<xml_diff>
--- a/Testing/Paretobranchfit_returned_parameters.xlsx
+++ b/Testing/Paretobranchfit_returned_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Studium\Masterarbeit\git\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Fabian/OneDrive/Studium/Masterarbeit/git/Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="11_AD4DB114E441178AC67DF4CD5690C74E693EDF1D" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{7F6E9E33-F2FD-4893-94CC-1F4B0A764E4D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FF065B-6E4B-554F-B518-CBFD03DD595E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="37">
   <si>
     <t>Pareto</t>
   </si>
@@ -112,13 +112,37 @@
   </si>
   <si>
     <t>--</t>
+  </si>
+  <si>
+    <t>p_cilo</t>
+  </si>
+  <si>
+    <t>p_cihi</t>
+  </si>
+  <si>
+    <t>q_cilo</t>
+  </si>
+  <si>
+    <t>q_cihi</t>
+  </si>
+  <si>
+    <t>a_cilo</t>
+  </si>
+  <si>
+    <t>a_cihi</t>
+  </si>
+  <si>
+    <t>c_cilo</t>
+  </si>
+  <si>
+    <t>c_cihi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +163,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -210,9 +240,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -222,6 +249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -502,40 +530,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:AE18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="10">
+      <c r="B1" s="9">
         <v>0</v>
       </c>
       <c r="C1" s="2">
@@ -601,12 +629,36 @@
       <c r="W1" s="2">
         <v>21</v>
       </c>
+      <c r="X1" s="2">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="2">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="2">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="2">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="2">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="2">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="2">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="2">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -655,15 +707,15 @@
         <v>25</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="U2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="U2" s="5" t="s">
         <v>28</v>
       </c>
       <c r="V2" s="6" t="s">
@@ -672,12 +724,36 @@
       <c r="W2" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="X2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -731,24 +807,48 @@
       <c r="S3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="T3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="U3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="V3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="W3" s="9" t="s">
+      <c r="T3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="V3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -808,18 +908,42 @@
       <c r="U4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="V4" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="W4" s="9" t="s">
+      <c r="V4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="W4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="X4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE4" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -885,8 +1009,32 @@
       <c r="W5" s="8" t="s">
         <v>25</v>
       </c>
+      <c r="X5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE5" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -910,6 +1058,16 @@
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
     </row>
+    <row r="17" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P17" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P18" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
prep_table update #2 for CIs
</commit_message>
<xml_diff>
--- a/Testing/Paretobranchfit_returned_parameters.xlsx
+++ b/Testing/Paretobranchfit_returned_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Fabian/OneDrive/Studium/Masterarbeit/git/Testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Studium\Masterarbeit\git\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FF065B-6E4B-554F-B518-CBFD03DD595E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{8FFD3452-E927-4970-8FF5-B16CE6CE8405}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -142,7 +142,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,34 +532,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -654,7 +654,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -749,7 +749,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -844,7 +844,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -939,7 +939,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1058,12 +1058,12 @@
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
     </row>
-    <row r="17" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="16:16">
       <c r="P17" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="16:16">
       <c r="P18" s="12" t="s">
         <v>30</v>
       </c>

</xml_diff>